<commit_message>
Opción para importar stock en bodegas diferentes de la principal
</commit_message>
<xml_diff>
--- a/public/plantilla_importar_stock_cajs.xlsx
+++ b/public/plantilla_importar_stock_cajs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\almacengt\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603AAD0D-3AA0-40A1-B4D9-0A2A92718F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7703D8D3-D78A-4701-9608-C185983C08B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7AB58512-C261-4305-B6E4-31B8102C15CE}"/>
   </bookViews>
@@ -510,7 +510,7 @@
         <v>75</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -530,7 +530,7 @@
         <v>42</v>
       </c>
       <c r="F3">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>